<commit_message>
Add PDF and Excel fixture files for testing purposes
- Created a new PDF file 'documento_rir_B.pdf' with generated content.
- Added a new Excel file 'manifesto_completo.xlsx' containing multiple sheets and properties.
</commit_message>
<xml_diff>
--- a/tests/fixtures/manifesto_exemplo.xlsx
+++ b/tests/fixtures/manifesto_exemplo.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D3"/>
+  <dimension ref="A1:I3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -439,14 +439,39 @@
       </c>
       <c r="D1" t="inlineStr">
         <is>
+          <t>ARQUIVO</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>FORMATO</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
           <t>DISCIPLINA</t>
+        </is>
+      </c>
+      <c r="G1" t="inlineStr">
+        <is>
+          <t>TIPO DE DOCUMENTO</t>
+        </is>
+      </c>
+      <c r="H1" t="inlineStr">
+        <is>
+          <t>PROPÓSITO</t>
+        </is>
+      </c>
+      <c r="I1" t="inlineStr">
+        <is>
+          <t>CAMINHO DATABOOK</t>
         </is>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>DOC-001-TEST</t>
+          <t>documento_pid</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
@@ -456,19 +481,40 @@
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>Documento de Teste Um</t>
-        </is>
-      </c>
-      <c r="D2" t="inlineStr">
-        <is>
-          <t>ENGENHARIA</t>
+          <t>Documento PID de Teste</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr"/>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>A4</t>
+        </is>
+      </c>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>PROCESSO</t>
+        </is>
+      </c>
+      <c r="G2" t="inlineStr">
+        <is>
+          <t>PID</t>
+        </is>
+      </c>
+      <c r="H2" t="inlineStr">
+        <is>
+          <t>Para Construção</t>
+        </is>
+      </c>
+      <c r="I2" t="inlineStr">
+        <is>
+          <t>DATA BOOK C&amp;M</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>DOC-002-TEST</t>
+          <t>documento_rir</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
@@ -478,12 +524,33 @@
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>Documento de Teste Dois</t>
-        </is>
-      </c>
-      <c r="D3" t="inlineStr">
-        <is>
-          <t>CIVIL</t>
+          <t>Documento RIR de Teste</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr"/>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>A3</t>
+        </is>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>INSTRUMENTAÇÃO</t>
+        </is>
+      </c>
+      <c r="G3" t="inlineStr">
+        <is>
+          <t>RIR</t>
+        </is>
+      </c>
+      <c r="H3" t="inlineStr">
+        <is>
+          <t>Para Construção</t>
+        </is>
+      </c>
+      <c r="I3" t="inlineStr">
+        <is>
+          <t>DATA BOOK C&amp;M</t>
         </is>
       </c>
     </row>

</xml_diff>